<commit_message>
Edit customDiceOutcomes to be more intuitive
</commit_message>
<xml_diff>
--- a/customDiceOutcomes.xlsx
+++ b/customDiceOutcomes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni\Python\WildMagic\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thias\Documents\GitHub\wildmagic-roller\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EC7BB20-A444-42BE-969C-E7F5824F264E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD2AEB63-9E3D-4322-810C-E3E35B5F1283}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="43">
   <si>
     <t>Dierolls</t>
   </si>
@@ -85,9 +85,6 @@
     <t>GoTo</t>
   </si>
   <si>
-    <t>Table 1</t>
-  </si>
-  <si>
     <t>Table 2</t>
   </si>
   <si>
@@ -118,9 +115,6 @@
     <t>Except</t>
   </si>
   <si>
-    <t>2, 3</t>
-  </si>
-  <si>
     <t>Table 3</t>
   </si>
   <si>
@@ -130,7 +124,43 @@
     <t>Outcome 14</t>
   </si>
   <si>
-    <t>The "Except" column is for when a table is declared in the GoTo column. If certain rolls on the chosen table are to be ignored, they are to be written comma-sepperated (num1, num2, num3…) in the Except column.</t>
+    <t>Main Table</t>
+  </si>
+  <si>
+    <t>Table 4</t>
+  </si>
+  <si>
+    <t>Table 5</t>
+  </si>
+  <si>
+    <t>Outcome 15</t>
+  </si>
+  <si>
+    <t>Outcome 16</t>
+  </si>
+  <si>
+    <t>Outcome 17</t>
+  </si>
+  <si>
+    <t>Outcome 18</t>
+  </si>
+  <si>
+    <t>Table 2, Table 3</t>
+  </si>
+  <si>
+    <t>5-7, 9-10</t>
+  </si>
+  <si>
+    <t>Example Table</t>
+  </si>
+  <si>
+    <t>The "Except" column is for when a table is declared in the GoTo column. If certain (ranges of) rolls on the chosen table are to be ignored, they are to be written comma-separated (num1, num2, num3…) in the Except column.</t>
+  </si>
+  <si>
+    <t>1, 2-90</t>
+  </si>
+  <si>
+    <t>0, 1-10</t>
   </si>
 </sst>
 </file>
@@ -486,7 +516,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
+        <fgColor rgb="FFBFBFBF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -832,10 +862,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -874,6 +909,12 @@
     <xf numFmtId="0" fontId="19" fillId="34" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -883,20 +924,11 @@
     <xf numFmtId="0" fontId="0" fillId="35" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -947,6 +979,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFBFBFBF"/>
       <color rgb="FFCC0000"/>
     </mruColors>
   </colors>
@@ -1258,24 +1291,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L62"/>
+  <dimension ref="A1:R62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34:D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16" customWidth="1"/>
     <col min="10" max="10" width="6.6640625" customWidth="1"/>
     <col min="11" max="11" width="4" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="6.6640625" customWidth="1"/>
+    <col min="14" max="14" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1283,109 +1319,157 @@
       <c r="C1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="25" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E1" s="24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="4">
         <v>1</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" s="46"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D2" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="25"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="4">
         <v>10</v>
       </c>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="45"/>
-    </row>
-    <row r="4" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="40"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="25"/>
+    </row>
+    <row r="4" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6"/>
       <c r="B4" s="15"/>
       <c r="C4" s="14"/>
       <c r="D4" s="20"/>
       <c r="E4" s="15"/>
-      <c r="G4" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" s="34"/>
-      <c r="I4" s="34"/>
-      <c r="J4" s="34"/>
-      <c r="K4" s="34"/>
-      <c r="L4" s="35"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G4" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="35"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="35"/>
+      <c r="K4" s="35"/>
+      <c r="L4" s="36"/>
+      <c r="N4" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="P4" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="R4" s="24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="11">
         <v>11</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="26"/>
-      <c r="E5" s="46"/>
-      <c r="G5" s="36"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="37"/>
-      <c r="J5" s="37"/>
-      <c r="K5" s="37"/>
-      <c r="L5" s="38"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D5" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="26"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="38"/>
+      <c r="J5" s="38"/>
+      <c r="K5" s="38"/>
+      <c r="L5" s="39"/>
+      <c r="N5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="O5" s="4">
+        <v>1</v>
+      </c>
+      <c r="P5" s="40" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q5" s="41" t="s">
+        <v>37</v>
+      </c>
+      <c r="R5" s="26" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="12">
         <v>20</v>
       </c>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="45"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="27"/>
       <c r="G6" s="10"/>
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
       <c r="J6" s="10"/>
       <c r="K6" s="10"/>
       <c r="L6" s="10"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="N6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="O6" s="4">
+        <v>10</v>
+      </c>
+      <c r="P6" s="40"/>
+      <c r="Q6" s="41"/>
+      <c r="R6" s="27"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="6"/>
       <c r="B7" s="21"/>
       <c r="C7" s="14"/>
       <c r="D7" s="20"/>
       <c r="E7" s="15"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="N7" s="6"/>
+      <c r="O7" s="15"/>
+      <c r="P7" s="14"/>
+      <c r="Q7" s="20"/>
+      <c r="R7" s="15"/>
+    </row>
+    <row r="8" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="13">
         <v>21</v>
       </c>
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="26"/>
-      <c r="E8" s="46"/>
+      <c r="D8" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="26"/>
       <c r="G8" s="5" t="s">
         <v>14</v>
       </c>
@@ -1394,140 +1478,214 @@
       <c r="J8" s="8"/>
       <c r="K8" s="8"/>
       <c r="L8" s="9"/>
-    </row>
-    <row r="9" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="O8" s="11">
+        <v>11</v>
+      </c>
+      <c r="P8" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q8" s="40"/>
+      <c r="R8" s="26"/>
+    </row>
+    <row r="9" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="13">
         <v>30</v>
       </c>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="45"/>
-      <c r="G9" s="27" t="s">
+      <c r="C9" s="40"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="27"/>
+      <c r="G9" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="H9" s="28"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="28"/>
-      <c r="K9" s="28"/>
-      <c r="L9" s="29"/>
-    </row>
-    <row r="10" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H9" s="29"/>
+      <c r="I9" s="29"/>
+      <c r="J9" s="29"/>
+      <c r="K9" s="29"/>
+      <c r="L9" s="30"/>
+      <c r="N9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="O9" s="12">
+        <v>20</v>
+      </c>
+      <c r="P9" s="40"/>
+      <c r="Q9" s="40"/>
+      <c r="R9" s="27"/>
+    </row>
+    <row r="10" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6"/>
       <c r="B10" s="21"/>
       <c r="C10" s="14"/>
       <c r="D10" s="20"/>
       <c r="E10" s="15"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="31"/>
-      <c r="I10" s="31"/>
-      <c r="J10" s="31"/>
-      <c r="K10" s="31"/>
-      <c r="L10" s="32"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G10" s="31"/>
+      <c r="H10" s="32"/>
+      <c r="I10" s="32"/>
+      <c r="J10" s="32"/>
+      <c r="K10" s="32"/>
+      <c r="L10" s="33"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="21"/>
+      <c r="P10" s="14"/>
+      <c r="Q10" s="20"/>
+      <c r="R10" s="15"/>
+    </row>
+    <row r="11" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B11" s="13">
         <v>31</v>
       </c>
-      <c r="C11" s="26" t="s">
+      <c r="C11" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="26"/>
-      <c r="E11" s="46"/>
-      <c r="G11" s="30"/>
-      <c r="H11" s="31"/>
-      <c r="I11" s="31"/>
-      <c r="J11" s="31"/>
-      <c r="K11" s="31"/>
-      <c r="L11" s="32"/>
-    </row>
-    <row r="12" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D11" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="26"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="32"/>
+      <c r="K11" s="32"/>
+      <c r="L11" s="33"/>
+      <c r="N11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="O11" s="13">
+        <v>21</v>
+      </c>
+      <c r="P11" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q11" s="40"/>
+      <c r="R11" s="26"/>
+    </row>
+    <row r="12" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B12" s="13">
         <v>40</v>
       </c>
-      <c r="C12" s="26"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="45"/>
-      <c r="G12" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="H12" s="31"/>
-      <c r="I12" s="31"/>
-      <c r="J12" s="31"/>
-      <c r="K12" s="31"/>
-      <c r="L12" s="32"/>
-    </row>
-    <row r="13" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="40"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="27"/>
+      <c r="G12" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" s="32"/>
+      <c r="I12" s="32"/>
+      <c r="J12" s="32"/>
+      <c r="K12" s="32"/>
+      <c r="L12" s="33"/>
+      <c r="N12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="O12" s="13">
+        <v>30</v>
+      </c>
+      <c r="P12" s="40"/>
+      <c r="Q12" s="40"/>
+      <c r="R12" s="27"/>
+    </row>
+    <row r="13" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6"/>
       <c r="B13" s="21"/>
       <c r="C13" s="14"/>
       <c r="D13" s="20"/>
       <c r="E13" s="15"/>
-      <c r="G13" s="30"/>
-      <c r="H13" s="31"/>
-      <c r="I13" s="31"/>
-      <c r="J13" s="31"/>
-      <c r="K13" s="31"/>
-      <c r="L13" s="32"/>
-    </row>
-    <row r="14" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G13" s="31"/>
+      <c r="H13" s="32"/>
+      <c r="I13" s="32"/>
+      <c r="J13" s="32"/>
+      <c r="K13" s="32"/>
+      <c r="L13" s="33"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="21"/>
+      <c r="P13" s="14"/>
+      <c r="Q13" s="20"/>
+      <c r="R13" s="15"/>
+    </row>
+    <row r="14" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B14" s="13">
         <v>41</v>
       </c>
-      <c r="C14" s="26" t="s">
+      <c r="C14" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="26"/>
-      <c r="E14" s="46"/>
-      <c r="G14" s="30"/>
-      <c r="H14" s="31"/>
-      <c r="I14" s="31"/>
-      <c r="J14" s="31"/>
-      <c r="K14" s="31"/>
-      <c r="L14" s="32"/>
-    </row>
-    <row r="15" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D14" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="26"/>
+      <c r="G14" s="31"/>
+      <c r="H14" s="32"/>
+      <c r="I14" s="32"/>
+      <c r="J14" s="32"/>
+      <c r="K14" s="32"/>
+      <c r="L14" s="33"/>
+      <c r="N14" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="O14" s="13">
+        <v>31</v>
+      </c>
+      <c r="P14" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q14" s="40"/>
+      <c r="R14" s="26"/>
+    </row>
+    <row r="15" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B15" s="13">
         <v>50</v>
       </c>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="45"/>
-      <c r="G15" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="H15" s="31"/>
-      <c r="I15" s="31"/>
-      <c r="J15" s="31"/>
-      <c r="K15" s="31"/>
-      <c r="L15" s="32"/>
-    </row>
-    <row r="16" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C15" s="40"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="27"/>
+      <c r="G15" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="H15" s="32"/>
+      <c r="I15" s="32"/>
+      <c r="J15" s="32"/>
+      <c r="K15" s="32"/>
+      <c r="L15" s="33"/>
+      <c r="N15" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="O15" s="13">
+        <v>40</v>
+      </c>
+      <c r="P15" s="40"/>
+      <c r="Q15" s="40"/>
+      <c r="R15" s="27"/>
+    </row>
+    <row r="16" spans="1:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6"/>
       <c r="B16" s="21"/>
       <c r="C16" s="14"/>
       <c r="D16" s="20"/>
       <c r="E16" s="15"/>
-      <c r="G16" s="39"/>
-      <c r="H16" s="40"/>
-      <c r="I16" s="40"/>
-      <c r="J16" s="40"/>
-      <c r="K16" s="40"/>
-      <c r="L16" s="41"/>
+      <c r="G16" s="42"/>
+      <c r="H16" s="43"/>
+      <c r="I16" s="43"/>
+      <c r="J16" s="43"/>
+      <c r="K16" s="43"/>
+      <c r="L16" s="44"/>
     </row>
     <row r="17" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
@@ -1536,11 +1694,13 @@
       <c r="B17" s="13">
         <v>51</v>
       </c>
-      <c r="C17" s="26" t="s">
+      <c r="C17" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="D17" s="26"/>
-      <c r="E17" s="46"/>
+      <c r="D17" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="26"/>
     </row>
     <row r="18" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
@@ -1549,17 +1709,17 @@
       <c r="B18" s="13">
         <v>60</v>
       </c>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="45"/>
-      <c r="G18" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
-      <c r="K18" s="42"/>
-      <c r="L18" s="42"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="27"/>
+      <c r="G18" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="H18" s="25"/>
+      <c r="I18" s="25"/>
+      <c r="J18" s="25"/>
+      <c r="K18" s="25"/>
+      <c r="L18" s="25"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="6"/>
@@ -1567,31 +1727,33 @@
       <c r="C19" s="14"/>
       <c r="D19" s="20"/>
       <c r="E19" s="15"/>
-      <c r="G19" s="42"/>
-      <c r="H19" s="42"/>
-      <c r="I19" s="42"/>
-      <c r="J19" s="42"/>
-      <c r="K19" s="42"/>
-      <c r="L19" s="42"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G19" s="25"/>
+      <c r="H19" s="25"/>
+      <c r="I19" s="25"/>
+      <c r="J19" s="25"/>
+      <c r="K19" s="25"/>
+      <c r="L19" s="25"/>
+    </row>
+    <row r="20" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B20" s="13">
         <v>61</v>
       </c>
-      <c r="C20" s="26" t="s">
+      <c r="C20" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="D20" s="26"/>
-      <c r="E20" s="46"/>
-      <c r="G20" s="42"/>
-      <c r="H20" s="42"/>
-      <c r="I20" s="42"/>
-      <c r="J20" s="42"/>
-      <c r="K20" s="42"/>
-      <c r="L20" s="42"/>
+      <c r="D20" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" s="26"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="25"/>
+      <c r="I20" s="25"/>
+      <c r="J20" s="25"/>
+      <c r="K20" s="25"/>
+      <c r="L20" s="25"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
@@ -1600,15 +1762,15 @@
       <c r="B21" s="13">
         <v>70</v>
       </c>
-      <c r="C21" s="26"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="45"/>
-      <c r="G21" s="42"/>
-      <c r="H21" s="42"/>
-      <c r="I21" s="42"/>
-      <c r="J21" s="42"/>
-      <c r="K21" s="42"/>
-      <c r="L21" s="42"/>
+      <c r="C21" s="40"/>
+      <c r="D21" s="41"/>
+      <c r="E21" s="27"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="25"/>
+      <c r="I21" s="25"/>
+      <c r="J21" s="25"/>
+      <c r="K21" s="25"/>
+      <c r="L21" s="25"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="6"/>
@@ -1617,18 +1779,20 @@
       <c r="D22" s="20"/>
       <c r="E22" s="15"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B23" s="13">
         <v>71</v>
       </c>
-      <c r="C23" s="26" t="s">
+      <c r="C23" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="D23" s="26"/>
-      <c r="E23" s="46"/>
+      <c r="D23" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23" s="26"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
@@ -1637,9 +1801,9 @@
       <c r="B24" s="13">
         <v>80</v>
       </c>
-      <c r="C24" s="26"/>
-      <c r="D24" s="26"/>
-      <c r="E24" s="45"/>
+      <c r="C24" s="40"/>
+      <c r="D24" s="41"/>
+      <c r="E24" s="27"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="6"/>
@@ -1648,18 +1812,20 @@
       <c r="D25" s="20"/>
       <c r="E25" s="15"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B26" s="13">
         <v>81</v>
       </c>
-      <c r="C26" s="26" t="s">
+      <c r="C26" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="D26" s="26"/>
-      <c r="E26" s="46"/>
+      <c r="D26" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="E26" s="26"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
@@ -1668,9 +1834,9 @@
       <c r="B27" s="13">
         <v>90</v>
       </c>
-      <c r="C27" s="26"/>
-      <c r="D27" s="26"/>
-      <c r="E27" s="45"/>
+      <c r="C27" s="40"/>
+      <c r="D27" s="41"/>
+      <c r="E27" s="27"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="6"/>
@@ -1679,18 +1845,22 @@
       <c r="D28" s="20"/>
       <c r="E28" s="15"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B29" s="13">
         <v>91</v>
       </c>
-      <c r="C29" s="26" t="s">
+      <c r="C29" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="D29" s="26"/>
-      <c r="E29" s="46"/>
+      <c r="D29" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="E29" s="26" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
@@ -1699,9 +1869,9 @@
       <c r="B30" s="13">
         <v>100</v>
       </c>
-      <c r="C30" s="26"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="45"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="41"/>
+      <c r="E30" s="27"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="7"/>
@@ -1717,7 +1887,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>0</v>
@@ -1728,8 +1898,8 @@
       <c r="D33" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E33" s="23" t="s">
-        <v>27</v>
+      <c r="E33" s="24" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
@@ -1739,11 +1909,15 @@
       <c r="B34" s="4">
         <v>5</v>
       </c>
-      <c r="C34" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="D34" s="26"/>
-      <c r="E34" s="46"/>
+      <c r="C34" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="D34" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="E34" s="26" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
@@ -1752,9 +1926,9 @@
       <c r="B35" s="4">
         <v>10</v>
       </c>
-      <c r="C35" s="26"/>
-      <c r="D35" s="26"/>
-      <c r="E35" s="45"/>
+      <c r="C35" s="40"/>
+      <c r="D35" s="40"/>
+      <c r="E35" s="27"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="6"/>
@@ -1770,11 +1944,15 @@
       <c r="B37" s="11">
         <v>11</v>
       </c>
-      <c r="C37" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="D37" s="26"/>
-      <c r="E37" s="46"/>
+      <c r="C37" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="D37" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="E37" s="26" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
@@ -1783,9 +1961,9 @@
       <c r="B38" s="12">
         <v>20</v>
       </c>
-      <c r="C38" s="26"/>
-      <c r="D38" s="26"/>
-      <c r="E38" s="45"/>
+      <c r="C38" s="40"/>
+      <c r="D38" s="40"/>
+      <c r="E38" s="27"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B39" s="1"/>
@@ -1798,7 +1976,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="18" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>0</v>
@@ -1809,8 +1987,8 @@
       <c r="D41" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E41" s="23" t="s">
-        <v>27</v>
+      <c r="E41" s="24" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
@@ -1820,13 +1998,15 @@
       <c r="B42" s="4">
         <v>3</v>
       </c>
-      <c r="C42" s="26" t="s">
+      <c r="C42" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="D42" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="D42" s="26">
-        <v>1</v>
-      </c>
-      <c r="E42" s="46"/>
+      <c r="E42" s="26" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
@@ -1835,9 +2015,9 @@
       <c r="B43" s="4">
         <v>8</v>
       </c>
-      <c r="C43" s="26"/>
-      <c r="D43" s="26"/>
-      <c r="E43" s="45"/>
+      <c r="C43" s="40"/>
+      <c r="D43" s="40"/>
+      <c r="E43" s="27"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="6"/>
@@ -1853,13 +2033,15 @@
       <c r="B45" s="11">
         <v>9</v>
       </c>
-      <c r="C45" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="D45" s="26">
-        <v>1</v>
-      </c>
-      <c r="E45" s="46"/>
+      <c r="C45" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="D45" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="E45" s="26" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
@@ -1868,9 +2050,9 @@
       <c r="B46" s="12">
         <v>53</v>
       </c>
-      <c r="C46" s="26"/>
-      <c r="D46" s="26"/>
-      <c r="E46" s="45"/>
+      <c r="C46" s="40"/>
+      <c r="D46" s="40"/>
+      <c r="E46" s="27"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C47"/>
@@ -1878,64 +2060,207 @@
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C48"/>
     </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C49"/>
-    </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C50"/>
-    </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C51"/>
-    </row>
-    <row r="52" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C52"/>
-    </row>
-    <row r="53" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C53"/>
-    </row>
-    <row r="54" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C54"/>
-    </row>
-    <row r="55" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C49" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="D49" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E49" s="24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B50" s="4">
+        <v>3</v>
+      </c>
+      <c r="C50" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="D50" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="E50" s="26"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B51" s="4">
+        <v>8</v>
+      </c>
+      <c r="C51" s="40"/>
+      <c r="D51" s="40"/>
+      <c r="E51" s="27"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" s="6"/>
+      <c r="B52" s="15"/>
+      <c r="C52" s="14"/>
+      <c r="D52" s="20"/>
+      <c r="E52" s="15"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B53" s="11">
+        <v>9</v>
+      </c>
+      <c r="C53" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="D53" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="E53" s="26"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B54" s="12">
+        <v>53</v>
+      </c>
+      <c r="C54" s="40"/>
+      <c r="D54" s="40"/>
+      <c r="E54" s="27"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C55"/>
     </row>
-    <row r="56" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C56"/>
     </row>
-    <row r="57" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C57"/>
-    </row>
-    <row r="58" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C58"/>
-    </row>
-    <row r="59" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C59"/>
-    </row>
-    <row r="60" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C60"/>
-    </row>
-    <row r="61" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C61"/>
-    </row>
-    <row r="62" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C62"/>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C57" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="D57" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E57" s="24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B58" s="4">
+        <v>3</v>
+      </c>
+      <c r="C58" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="D58" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="E58" s="26"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B59" s="4">
+        <v>8</v>
+      </c>
+      <c r="C59" s="40"/>
+      <c r="D59" s="40"/>
+      <c r="E59" s="27"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60" s="6"/>
+      <c r="B60" s="15"/>
+      <c r="C60" s="14"/>
+      <c r="D60" s="20"/>
+      <c r="E60" s="15"/>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A61" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B61" s="11">
+        <v>9</v>
+      </c>
+      <c r="C61" s="40" t="s">
+        <v>36</v>
+      </c>
+      <c r="D61" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="E61" s="26"/>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A62" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B62" s="12">
+        <v>53</v>
+      </c>
+      <c r="C62" s="40"/>
+      <c r="D62" s="40"/>
+      <c r="E62" s="27"/>
     </row>
   </sheetData>
-  <mergeCells count="47">
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="E42:E43"/>
-    <mergeCell ref="E45:E46"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="E14:E15"/>
+  <mergeCells count="71">
+    <mergeCell ref="P14:P15"/>
+    <mergeCell ref="Q14:Q15"/>
+    <mergeCell ref="R14:R15"/>
+    <mergeCell ref="P8:P9"/>
+    <mergeCell ref="Q8:Q9"/>
+    <mergeCell ref="R8:R9"/>
+    <mergeCell ref="P11:P12"/>
+    <mergeCell ref="Q11:Q12"/>
+    <mergeCell ref="R11:R12"/>
+    <mergeCell ref="P5:P6"/>
+    <mergeCell ref="Q5:Q6"/>
+    <mergeCell ref="R5:R6"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="E58:E59"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="C61:C62"/>
+    <mergeCell ref="D61:D62"/>
+    <mergeCell ref="E61:E62"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="E50:E51"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="E53:E54"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="C20:C21"/>
     <mergeCell ref="G9:L11"/>
     <mergeCell ref="G4:L5"/>
     <mergeCell ref="C5:C6"/>
@@ -1952,23 +2277,20 @@
     <mergeCell ref="G18:L21"/>
     <mergeCell ref="C23:C24"/>
     <mergeCell ref="C26:C27"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="E42:E43"/>
+    <mergeCell ref="E45:E46"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="E14:E15"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1981,7 +2303,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1992,24 +2314,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
         <v>25</v>
       </c>
-      <c r="B1" t="s">
-        <v>26</v>
-      </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="43" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="44">
+      <c r="A2" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="46">
         <v>20</v>
       </c>
       <c r="C2" s="22"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="43"/>
-      <c r="B3" s="44"/>
+      <c r="A3" s="45"/>
+      <c r="B3" s="46"/>
       <c r="C3" s="22"/>
     </row>
   </sheetData>

</xml_diff>